<commit_message>
new iq tests' answers
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB84439-09CE-43AD-BB12-56560A6C4CDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912BFD39-4A9D-41BD-868A-9B36886A7EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,24 +553,24 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
new Q8 pictures uploaded
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912BFD39-4A9D-41BD-868A-9B36886A7EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7235EE-9E17-4D78-8160-B7AA850C2F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for product session 2
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F304B02A-EE0E-4769-81A7-89C8F2E046D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5DC3FE-A984-4AD6-8096-BC7EA56919A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
use sample 1 for session today
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5DC3FE-A984-4AD6-8096-BC7EA56919A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE8CD78-E788-4D81-AD5C-A708E0BCA5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
change q2 for sample 4
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE8CD78-E788-4D81-AD5C-A708E0BCA5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F91651-A414-4457-AEE0-8F4B13AF4ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -463,12 +463,12 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 10/18/2021
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F91651-A414-4457-AEE0-8F4B13AF4ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37867E7C-1CDC-4D61-B04E-957FFBAC8DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for 10/19/2021 session
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37867E7C-1CDC-4D61-B04E-957FFBAC8DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B529FC7A-A257-4015-B0A7-7E6CF2F06490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
new sample for today's session
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B529FC7A-A257-4015-B0A7-7E6CF2F06490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0833ED3-D423-45B0-A71F-1D35B026BF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
+    <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
change of q7 and q10 for sample 4
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0833ED3-D423-45B0-A71F-1D35B026BF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DA86FB-632A-460C-9D8A-4F989640AD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -548,12 +548,12 @@
         <v>8</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -599,7 +599,7 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sample for session 10/20/2021
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DA86FB-632A-460C-9D8A-4F989640AD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AC77DC-A291-4440-8A56-1D472113B9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for sessions on 10/21/2021
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AC77DC-A291-4440-8A56-1D472113B9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79C383C-6D16-4F91-96C6-797E4F72CFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 10/22/2021_1
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79C383C-6D16-4F91-96C6-797E4F72CFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E4A0E9-C6AA-4232-AB7C-26007ADAA504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 10/22/2021_2
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E4A0E9-C6AA-4232-AB7C-26007ADAA504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456126F1-0FB1-4EDF-8FF7-0B7FDAB82D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 11/02/2021
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456126F1-0FB1-4EDF-8FF7-0B7FDAB82D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE80B3D-2C4C-47C4-B8F5-D5EED7D09FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
+    <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 11_05_2021
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE80B3D-2C4C-47C4-B8F5-D5EED7D09FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4384B1-9334-4A89-AE00-377FD66E8F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 11/10/2021
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4384B1-9334-4A89-AE00-377FD66E8F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F3FA90-F7CA-4E96-88D4-B8C7CB13EFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 11/12/2021
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F3FA90-F7CA-4E96-88D4-B8C7CB13EFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605599EB-E62F-44CF-988B-9EC39E69E434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
+    <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 11/17/2021
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605599EB-E62F-44CF-988B-9EC39E69E434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2003C6DF-06DF-47D2-8435-E931005A500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 11/18/2021
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2003C6DF-06DF-47D2-8435-E931005A500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2D34D7-6A9F-4878-AAFC-FE52A50396F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
iq sample for additional session1
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2D34D7-6A9F-4878-AAFC-FE52A50396F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6406D121-9B78-4E82-9A53-C5E6465BB2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
+    <workbookView xWindow="1500" yWindow="-13125" windowWidth="28800" windowHeight="11385" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for 02/02/2022 session
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6406D121-9B78-4E82-9A53-C5E6465BB2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E3E6DD-3C77-48DA-92F7-CF0D6A61220B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="-13125" windowWidth="28800" windowHeight="11385" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 02/03/2022
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C927EEC6-9AAC-4846-BB99-AACAF54A2859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CD4BAB-742B-474F-A0C4-CC3F45E63339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 02/04/2022
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CD4BAB-742B-474F-A0C4-CC3F45E63339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C025EA-EBF1-4115-A61F-988F4655D5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 02/04/2022 session
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C025EA-EBF1-4115-A61F-988F4655D5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1DFFB3-9EB3-45EB-AEF3-94F431287CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 02/05/2022
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1DFFB3-9EB3-45EB-AEF3-94F431287CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD39E35F-867A-4DE4-ABBC-D9E905054155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 02/06/2022
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD39E35F-867A-4DE4-ABBC-D9E905054155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ECA212-FEFC-4655-B09F-056620780ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>

<commit_message>
sample for session 02/07/2022
</commit_message>
<xml_diff>
--- a/configs/demo.xlsx
+++ b/configs/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwang\oTree\oTree\iq_test\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ECA212-FEFC-4655-B09F-056620780ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FD1401-0E09-4A8E-A6A7-05E47626E03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
+    <workbookView xWindow="-2850" yWindow="-14640" windowWidth="28800" windowHeight="11385" xr2:uid="{600702B7-CADF-46F9-B615-F6F46A6F771E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>6</v>

</xml_diff>